<commit_message>
Add button in mainmenu by using GUI SKIN
</commit_message>
<xml_diff>
--- a/Doc/Timeline Senior Project.xlsx
+++ b/Doc/Timeline Senior Project.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Function</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>SE testng</t>
+  </si>
+  <si>
+    <t>6 hrs</t>
+  </si>
+  <si>
+    <t>5 hrs</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +513,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,7 +794,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -793,11 +802,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK64"/>
+  <dimension ref="A1:AK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,233 +815,232 @@
     <col min="22" max="22" width="12.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="C1" s="43">
+        <v>41284</v>
+      </c>
+      <c r="D1" s="43">
+        <v>41285</v>
+      </c>
+      <c r="E1" s="43">
+        <v>41286</v>
+      </c>
+      <c r="F1" s="43">
+        <v>41287</v>
+      </c>
+      <c r="G1" s="43">
+        <v>41288</v>
+      </c>
+      <c r="H1" s="43">
+        <v>41289</v>
+      </c>
+      <c r="I1" s="43">
+        <v>41290</v>
+      </c>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="27">
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="O2" s="27">
         <v>41283</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="34">
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="34">
         <v>41302</v>
       </c>
-      <c r="W1" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="31">
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="O3" s="31">
         <v>41297</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="P3" s="30" t="s">
         <v>48</v>
-      </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="3"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="31">
-        <v>41304</v>
-      </c>
-      <c r="P3" s="30" t="s">
-        <v>49</v>
       </c>
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
-      <c r="U3" s="3"/>
+      <c r="U3" s="32"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="31">
+        <v>41304</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:37" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15">
         <v>41276</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I6" s="15">
         <v>41277</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J6" s="15">
         <v>41278</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K6" s="15">
         <v>41279</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L6" s="15">
         <v>41280</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M6" s="15">
         <v>41281</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N6" s="15">
         <v>41282</v>
       </c>
-      <c r="O5" s="26">
+      <c r="O6" s="26">
         <v>41283</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P6" s="15">
         <v>41284</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q6" s="15">
         <v>41285</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R6" s="15">
         <v>41286</v>
       </c>
-      <c r="S5" s="15">
+      <c r="S6" s="15">
         <v>41287</v>
       </c>
-      <c r="T5" s="15">
+      <c r="T6" s="15">
         <v>41288</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U6" s="15">
         <v>41289</v>
       </c>
-      <c r="V5" s="25">
+      <c r="V6" s="25">
         <v>41290</v>
       </c>
-      <c r="W5" s="15">
+      <c r="W6" s="15">
         <v>41291</v>
       </c>
-      <c r="X5" s="15">
+      <c r="X6" s="15">
         <v>41292</v>
       </c>
-      <c r="Y5" s="15">
+      <c r="Y6" s="15">
         <v>41293</v>
       </c>
-      <c r="Z5" s="15">
+      <c r="Z6" s="15">
         <v>41294</v>
       </c>
-      <c r="AA5" s="15">
+      <c r="AA6" s="15">
         <v>41295</v>
       </c>
-      <c r="AB5" s="15">
+      <c r="AB6" s="15">
         <v>41296</v>
       </c>
-      <c r="AC5" s="17">
+      <c r="AC6" s="17">
         <v>41297</v>
       </c>
-      <c r="AD5" s="15">
+      <c r="AD6" s="15">
         <v>41298</v>
       </c>
-      <c r="AE5" s="15">
+      <c r="AE6" s="15">
         <v>41299</v>
       </c>
-      <c r="AF5" s="15">
+      <c r="AF6" s="15">
         <v>41300</v>
       </c>
-      <c r="AG5" s="15">
+      <c r="AG6" s="15">
         <v>41301</v>
       </c>
-      <c r="AH5" s="15">
+      <c r="AH6" s="15">
         <v>41302</v>
       </c>
-      <c r="AI5" s="15">
+      <c r="AI6" s="15">
         <v>41303</v>
       </c>
-      <c r="AJ5" s="17">
+      <c r="AJ6" s="17">
         <v>41304</v>
       </c>
-      <c r="AK5" s="28">
+      <c r="AK6" s="28">
         <v>41305</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="7" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="5"/>
-    </row>
-    <row r="7" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>2</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1061,10 +1067,12 @@
       <c r="AJ7" s="4"/>
       <c r="AK7" s="5"/>
     </row>
-    <row r="8" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="21" t="s">
-        <v>55</v>
+    <row r="8" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1102,10 +1110,10 @@
       <c r="AJ8" s="4"/>
       <c r="AK8" s="5"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="21" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1126,7 +1134,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
-      <c r="V9" s="24"/>
+      <c r="V9" s="8"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -1146,18 +1154,18 @@
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1167,7 +1175,7 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
-      <c r="V10" s="8"/>
+      <c r="V10" s="24"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -1186,19 +1194,19 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
+      <c r="B11" s="21" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1228,7 +1236,7 @@
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1268,17 +1276,19 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1306,25 +1316,21 @@
       <c r="AK13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>38</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1349,9 +1355,11 @@
       <c r="AK14" s="5"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="16" t="s">
-        <v>22</v>
+      <c r="A15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1392,7 +1400,7 @@
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1433,7 +1441,7 @@
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1441,13 +1449,13 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -1471,31 +1479,31 @@
       <c r="AJ17" s="4"/>
       <c r="AK17" s="5"/>
     </row>
-    <row r="18" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
-      <c r="V18" s="40" t="s">
-        <v>41</v>
-      </c>
+      <c r="V18" s="8"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -1514,22 +1522,20 @@
     </row>
     <row r="19" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
-      <c r="B19" s="16" t="s">
-        <v>25</v>
-      </c>
+      <c r="B19" s="16"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -1537,7 +1543,7 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
@@ -1558,7 +1564,7 @@
     <row r="20" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1580,7 +1586,7 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
@@ -1601,7 +1607,7 @@
     <row r="21" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1623,7 +1629,7 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
@@ -1644,7 +1650,7 @@
     <row r="22" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1666,7 +1672,7 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
@@ -1687,7 +1693,7 @@
     <row r="23" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="16" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1709,7 +1715,7 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
@@ -1727,29 +1733,33 @@
       <c r="AJ23" s="4"/>
       <c r="AK23" s="5"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
-      <c r="V24" s="39"/>
+      <c r="V24" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
@@ -1767,12 +1777,8 @@
       <c r="AK24" s="5"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>29</v>
-      </c>
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1792,7 +1798,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
-      <c r="V25" s="8"/>
+      <c r="V25" s="39"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
@@ -1810,9 +1816,11 @@
       <c r="AK25" s="5"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="16" t="s">
-        <v>30</v>
+      <c r="A26" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1853,7 +1861,7 @@
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1892,11 +1900,9 @@
       <c r="AK27" s="5"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="A28" s="7"/>
       <c r="B28" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1935,8 +1941,12 @@
       <c r="AK28" s="5"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1975,9 +1985,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="16" t="s">
-        <v>36</v>
-      </c>
+      <c r="B30" s="16"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2017,7 +2025,7 @@
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2058,7 +2066,7 @@
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2099,7 +2107,7 @@
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2139,7 +2147,9 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="16"/>
+      <c r="B34" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2177,25 +2187,21 @@
       <c r="AK34" s="5"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>37</v>
-      </c>
+      <c r="A35" s="7"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="16"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -2220,9 +2226,11 @@
       <c r="AK35" s="5"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="16" t="s">
-        <v>39</v>
+      <c r="A36" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -2262,20 +2270,22 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="16"/>
+      <c r="B37" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
@@ -2301,22 +2311,20 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="22" t="s">
-        <v>40</v>
-      </c>
+      <c r="B38" s="16"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="38"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
@@ -2342,20 +2350,22 @@
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="22"/>
+      <c r="B39" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
-      <c r="O39" s="16"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
@@ -2381,9 +2391,7 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="22" t="s">
-        <v>51</v>
-      </c>
+      <c r="B40" s="22"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2423,7 +2431,7 @@
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2464,12 +2472,10 @@
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2507,10 +2513,12 @@
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2548,7 +2556,7 @@
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2588,7 +2596,9 @@
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="16"/>
+      <c r="B45" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2599,9 +2609,9 @@
       <c r="J45" s="16"/>
       <c r="K45" s="16"/>
       <c r="L45" s="16"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -2666,17 +2676,17 @@
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="4"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
@@ -2703,10 +2713,8 @@
       <c r="AJ47" s="4"/>
       <c r="AK47" s="5"/>
     </row>
-    <row r="48" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
-        <v>7</v>
-      </c>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -2744,13 +2752,11 @@
       <c r="AJ48" s="4"/>
       <c r="AK48" s="5"/>
     </row>
-    <row r="49" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>9</v>
-      </c>
+    <row r="49" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2787,10 +2793,12 @@
       <c r="AJ49" s="4"/>
       <c r="AK49" s="5"/>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="4" t="s">
-        <v>56</v>
+    <row r="50" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2831,7 +2839,7 @@
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="4" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2872,7 +2880,7 @@
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -2913,7 +2921,7 @@
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2953,7 +2961,9 @@
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
-      <c r="B54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -2990,13 +3000,9 @@
       <c r="AJ54" s="4"/>
       <c r="AK54" s="5"/>
     </row>
-    <row r="55" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>13</v>
-      </c>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -3033,10 +3039,12 @@
       <c r="AJ55" s="4"/>
       <c r="AK55" s="5"/>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="4" t="s">
-        <v>14</v>
+    <row r="56" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -3077,7 +3085,7 @@
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -3117,7 +3125,9 @@
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -3156,9 +3166,7 @@
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -3197,7 +3205,9 @@
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
-      <c r="B60" s="4"/>
+      <c r="B60" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -3351,44 +3361,83 @@
       <c r="AJ63" s="4"/>
       <c r="AK63" s="5"/>
     </row>
-    <row r="64" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11"/>
-      <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="11"/>
-      <c r="X64" s="11"/>
-      <c r="Y64" s="11"/>
-      <c r="Z64" s="11"/>
-      <c r="AA64" s="11"/>
-      <c r="AB64" s="11"/>
-      <c r="AC64" s="11"/>
-      <c r="AD64" s="11"/>
-      <c r="AE64" s="11"/>
-      <c r="AF64" s="11"/>
-      <c r="AG64" s="11"/>
-      <c r="AH64" s="11"/>
-      <c r="AI64" s="11"/>
-      <c r="AJ64" s="11"/>
-      <c r="AK64" s="12"/>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="8"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+      <c r="Z64" s="4"/>
+      <c r="AA64" s="4"/>
+      <c r="AB64" s="4"/>
+      <c r="AC64" s="4"/>
+      <c r="AD64" s="4"/>
+      <c r="AE64" s="4"/>
+      <c r="AF64" s="4"/>
+      <c r="AG64" s="4"/>
+      <c r="AH64" s="4"/>
+      <c r="AI64" s="4"/>
+      <c r="AJ64" s="4"/>
+      <c r="AK64" s="5"/>
+    </row>
+    <row r="65" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="11"/>
+      <c r="U65" s="11"/>
+      <c r="V65" s="23"/>
+      <c r="W65" s="11"/>
+      <c r="X65" s="11"/>
+      <c r="Y65" s="11"/>
+      <c r="Z65" s="11"/>
+      <c r="AA65" s="11"/>
+      <c r="AB65" s="11"/>
+      <c r="AC65" s="11"/>
+      <c r="AD65" s="11"/>
+      <c r="AE65" s="11"/>
+      <c r="AF65" s="11"/>
+      <c r="AG65" s="11"/>
+      <c r="AH65" s="11"/>
+      <c r="AI65" s="11"/>
+      <c r="AJ65" s="11"/>
+      <c r="AK65" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>